<commit_message>
Add layer functions into its own folder
</commit_message>
<xml_diff>
--- a/project1/confusion_matrices.xlsx
+++ b/project1/confusion_matrices.xlsx
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="889" uniqueCount="836">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1309" uniqueCount="836">
   <si>
     <t>True Classification</t>
   </si>
@@ -2588,7 +2588,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="128">
+  <borders count="288">
     <border>
       <left/>
       <right/>
@@ -2805,12 +2805,172 @@
     <border/>
     <border/>
     <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="131">
+  <cellXfs count="291">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="true"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="true" applyBorder="true"/>
@@ -2954,6 +3114,166 @@
     <xf numFmtId="22" fontId="0" fillId="0" borderId="125" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="126" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="127" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="128" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="129" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="130" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="131" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="132" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="133" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="134" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="135" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="136" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="137" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="138" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="139" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="140" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="141" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="142" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="143" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="144" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="145" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="146" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="147" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="148" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="149" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="150" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="151" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="152" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="153" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="154" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="155" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="156" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="157" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="158" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="159" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="160" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="161" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="162" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="163" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="164" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="165" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="166" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="167" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="168" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="169" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="170" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="171" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="172" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="173" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="174" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="175" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="176" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="177" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="178" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="179" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="180" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="181" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="182" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="183" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="184" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="185" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="186" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="187" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="188" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="189" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="190" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="191" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="192" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="193" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="194" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="195" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="196" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="197" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="198" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="199" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="200" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="201" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="202" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="203" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="204" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="205" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="206" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="207" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="208" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="209" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="210" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="211" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="212" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="213" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="214" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="215" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="216" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="217" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="218" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="219" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="220" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="221" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="222" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="223" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="224" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="225" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="226" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="227" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="228" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="229" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="230" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="231" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="232" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="233" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="234" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="235" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="236" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="237" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="238" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="239" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="240" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="241" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="242" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="243" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="244" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="245" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="246" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="247" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="248" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="249" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="250" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="251" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="252" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="253" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="254" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="255" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="256" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="257" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="258" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="259" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="260" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="261" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="262" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="263" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="264" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="265" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="266" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="267" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="268" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="269" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="270" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="271" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="272" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="273" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="274" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="275" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="276" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="277" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="278" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="279" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="280" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="281" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="282" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="283" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="284" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="285" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="286" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="287" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3294,7 +3614,7 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="211" t="s">
         <v>626</v>
       </c>
       <c r="C1" s="5" t="s">
@@ -3311,35 +3631,35 @@
       <c r="L1" s="7"/>
     </row>
     <row r="2">
-      <c r="C2" s="1" t="s">
-        <v>627</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>628</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>629</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>630</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>631</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>632</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>633</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>634</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>635</v>
-      </c>
-      <c r="L2" s="1" t="s">
-        <v>636</v>
+      <c r="C2" s="215" t="s">
+        <v>826</v>
+      </c>
+      <c r="D2" s="215" t="s">
+        <v>827</v>
+      </c>
+      <c r="E2" s="215" t="s">
+        <v>828</v>
+      </c>
+      <c r="F2" s="215" t="s">
+        <v>829</v>
+      </c>
+      <c r="G2" s="215" t="s">
+        <v>830</v>
+      </c>
+      <c r="H2" s="215" t="s">
+        <v>831</v>
+      </c>
+      <c r="I2" s="215" t="s">
+        <v>832</v>
+      </c>
+      <c r="J2" s="215" t="s">
+        <v>833</v>
+      </c>
+      <c r="K2" s="215" t="s">
+        <v>834</v>
+      </c>
+      <c r="L2" s="215" t="s">
+        <v>835</v>
       </c>
       <c r="N2" s="3" t="s">
         <v>4</v>
@@ -3353,8 +3673,8 @@
       <c r="A3" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>637</v>
+      <c r="B3" s="217" t="s">
+        <v>826</v>
       </c>
       <c r="C3" s="2">
         <v>531</v>
@@ -3396,8 +3716,8 @@
     </row>
     <row r="4">
       <c r="A4" s="9"/>
-      <c r="B4" s="1" t="s">
-        <v>638</v>
+      <c r="B4" s="217" t="s">
+        <v>827</v>
       </c>
       <c r="C4" s="1">
         <v>40</v>
@@ -3439,8 +3759,8 @@
     </row>
     <row r="5">
       <c r="A5" s="9"/>
-      <c r="B5" s="1" t="s">
-        <v>639</v>
+      <c r="B5" s="217" t="s">
+        <v>828</v>
       </c>
       <c r="C5" s="1">
         <v>87</v>
@@ -3475,8 +3795,8 @@
     </row>
     <row r="6">
       <c r="A6" s="9"/>
-      <c r="B6" s="1" t="s">
-        <v>640</v>
+      <c r="B6" s="217" t="s">
+        <v>829</v>
       </c>
       <c r="C6" s="1">
         <v>39</v>
@@ -3511,8 +3831,8 @@
     </row>
     <row r="7">
       <c r="A7" s="9"/>
-      <c r="B7" s="1" t="s">
-        <v>641</v>
+      <c r="B7" s="217" t="s">
+        <v>830</v>
       </c>
       <c r="C7" s="1">
         <v>53</v>
@@ -3547,8 +3867,8 @@
     </row>
     <row r="8">
       <c r="A8" s="9"/>
-      <c r="B8" s="1" t="s">
-        <v>642</v>
+      <c r="B8" s="217" t="s">
+        <v>831</v>
       </c>
       <c r="C8" s="1">
         <v>19</v>
@@ -3583,8 +3903,8 @@
     </row>
     <row r="9">
       <c r="A9" s="9"/>
-      <c r="B9" s="1" t="s">
-        <v>643</v>
+      <c r="B9" s="217" t="s">
+        <v>832</v>
       </c>
       <c r="C9" s="1">
         <v>10</v>
@@ -3619,8 +3939,8 @@
     </row>
     <row r="10">
       <c r="A10" s="9"/>
-      <c r="B10" s="1" t="s">
-        <v>644</v>
+      <c r="B10" s="217" t="s">
+        <v>833</v>
       </c>
       <c r="C10" s="1">
         <v>32</v>
@@ -3655,8 +3975,8 @@
     </row>
     <row r="11">
       <c r="A11" s="9"/>
-      <c r="B11" s="1" t="s">
-        <v>645</v>
+      <c r="B11" s="217" t="s">
+        <v>834</v>
       </c>
       <c r="C11" s="1">
         <v>192</v>
@@ -3691,8 +4011,8 @@
     </row>
     <row r="12">
       <c r="A12" s="10"/>
-      <c r="B12" s="1" t="s">
-        <v>646</v>
+      <c r="B12" s="217" t="s">
+        <v>835</v>
       </c>
       <c r="C12" s="1">
         <v>69</v>
@@ -3762,7 +4082,7 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="283" t="s">
         <v>815</v>
       </c>
       <c r="C1" s="5" t="s">
@@ -3779,35 +4099,35 @@
       <c r="L1" s="7"/>
     </row>
     <row r="2">
-      <c r="C2" s="1" t="s">
-        <v>816</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>817</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>818</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>819</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>820</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>821</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>822</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>823</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>824</v>
-      </c>
-      <c r="L2" s="1" t="s">
-        <v>825</v>
+      <c r="C2" s="287" t="s">
+        <v>826</v>
+      </c>
+      <c r="D2" s="287" t="s">
+        <v>827</v>
+      </c>
+      <c r="E2" s="287" t="s">
+        <v>828</v>
+      </c>
+      <c r="F2" s="287" t="s">
+        <v>829</v>
+      </c>
+      <c r="G2" s="287" t="s">
+        <v>830</v>
+      </c>
+      <c r="H2" s="287" t="s">
+        <v>831</v>
+      </c>
+      <c r="I2" s="287" t="s">
+        <v>832</v>
+      </c>
+      <c r="J2" s="287" t="s">
+        <v>833</v>
+      </c>
+      <c r="K2" s="287" t="s">
+        <v>834</v>
+      </c>
+      <c r="L2" s="287" t="s">
+        <v>835</v>
       </c>
       <c r="N2" s="3" t="s">
         <v>4</v>
@@ -3821,7 +4141,7 @@
       <c r="A3" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="289" t="s">
         <v>826</v>
       </c>
       <c r="C3" s="2">
@@ -3864,7 +4184,7 @@
     </row>
     <row r="4">
       <c r="A4" s="9"/>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="289" t="s">
         <v>827</v>
       </c>
       <c r="C4" s="1">
@@ -3907,7 +4227,7 @@
     </row>
     <row r="5">
       <c r="A5" s="9"/>
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="289" t="s">
         <v>828</v>
       </c>
       <c r="C5" s="1">
@@ -3943,7 +4263,7 @@
     </row>
     <row r="6">
       <c r="A6" s="9"/>
-      <c r="B6" s="1" t="s">
+      <c r="B6" s="289" t="s">
         <v>829</v>
       </c>
       <c r="C6" s="1">
@@ -3979,7 +4299,7 @@
     </row>
     <row r="7">
       <c r="A7" s="9"/>
-      <c r="B7" s="1" t="s">
+      <c r="B7" s="289" t="s">
         <v>830</v>
       </c>
       <c r="C7" s="1">
@@ -4015,7 +4335,7 @@
     </row>
     <row r="8">
       <c r="A8" s="9"/>
-      <c r="B8" s="1" t="s">
+      <c r="B8" s="289" t="s">
         <v>831</v>
       </c>
       <c r="C8" s="1">
@@ -4051,7 +4371,7 @@
     </row>
     <row r="9">
       <c r="A9" s="9"/>
-      <c r="B9" s="1" t="s">
+      <c r="B9" s="289" t="s">
         <v>832</v>
       </c>
       <c r="C9" s="1">
@@ -4087,7 +4407,7 @@
     </row>
     <row r="10">
       <c r="A10" s="9"/>
-      <c r="B10" s="1" t="s">
+      <c r="B10" s="289" t="s">
         <v>833</v>
       </c>
       <c r="C10" s="1">
@@ -4123,7 +4443,7 @@
     </row>
     <row r="11">
       <c r="A11" s="9"/>
-      <c r="B11" s="1" t="s">
+      <c r="B11" s="289" t="s">
         <v>834</v>
       </c>
       <c r="C11" s="1">
@@ -4159,7 +4479,7 @@
     </row>
     <row r="12">
       <c r="A12" s="10"/>
-      <c r="B12" s="1" t="s">
+      <c r="B12" s="289" t="s">
         <v>835</v>
       </c>
       <c r="C12" s="1">
@@ -4229,7 +4549,7 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="219" t="s">
         <v>647</v>
       </c>
       <c r="C1" s="5" t="s">
@@ -4246,35 +4566,35 @@
       <c r="L1" s="7"/>
     </row>
     <row r="2">
-      <c r="C2" s="1" t="s">
-        <v>648</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>649</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>650</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>651</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>652</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>653</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>654</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>655</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>656</v>
-      </c>
-      <c r="L2" s="1" t="s">
-        <v>657</v>
+      <c r="C2" s="223" t="s">
+        <v>826</v>
+      </c>
+      <c r="D2" s="223" t="s">
+        <v>827</v>
+      </c>
+      <c r="E2" s="223" t="s">
+        <v>828</v>
+      </c>
+      <c r="F2" s="223" t="s">
+        <v>829</v>
+      </c>
+      <c r="G2" s="223" t="s">
+        <v>830</v>
+      </c>
+      <c r="H2" s="223" t="s">
+        <v>831</v>
+      </c>
+      <c r="I2" s="223" t="s">
+        <v>832</v>
+      </c>
+      <c r="J2" s="223" t="s">
+        <v>833</v>
+      </c>
+      <c r="K2" s="223" t="s">
+        <v>834</v>
+      </c>
+      <c r="L2" s="223" t="s">
+        <v>835</v>
       </c>
       <c r="N2" s="3" t="s">
         <v>4</v>
@@ -4288,8 +4608,8 @@
       <c r="A3" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>658</v>
+      <c r="B3" s="225" t="s">
+        <v>826</v>
       </c>
       <c r="C3" s="2">
         <v>216</v>
@@ -4331,8 +4651,8 @@
     </row>
     <row r="4">
       <c r="A4" s="9"/>
-      <c r="B4" s="1" t="s">
-        <v>659</v>
+      <c r="B4" s="225" t="s">
+        <v>827</v>
       </c>
       <c r="C4" s="1">
         <v>72</v>
@@ -4374,8 +4694,8 @@
     </row>
     <row r="5">
       <c r="A5" s="9"/>
-      <c r="B5" s="1" t="s">
-        <v>660</v>
+      <c r="B5" s="225" t="s">
+        <v>828</v>
       </c>
       <c r="C5" s="1">
         <v>52</v>
@@ -4410,8 +4730,8 @@
     </row>
     <row r="6">
       <c r="A6" s="9"/>
-      <c r="B6" s="1" t="s">
-        <v>661</v>
+      <c r="B6" s="225" t="s">
+        <v>829</v>
       </c>
       <c r="C6" s="1">
         <v>25</v>
@@ -4446,8 +4766,8 @@
     </row>
     <row r="7">
       <c r="A7" s="9"/>
-      <c r="B7" s="1" t="s">
-        <v>662</v>
+      <c r="B7" s="225" t="s">
+        <v>830</v>
       </c>
       <c r="C7" s="1">
         <v>27</v>
@@ -4482,8 +4802,8 @@
     </row>
     <row r="8">
       <c r="A8" s="9"/>
-      <c r="B8" s="1" t="s">
-        <v>663</v>
+      <c r="B8" s="225" t="s">
+        <v>831</v>
       </c>
       <c r="C8" s="1">
         <v>19</v>
@@ -4518,8 +4838,8 @@
     </row>
     <row r="9">
       <c r="A9" s="9"/>
-      <c r="B9" s="1" t="s">
-        <v>664</v>
+      <c r="B9" s="225" t="s">
+        <v>832</v>
       </c>
       <c r="C9" s="1">
         <v>6</v>
@@ -4554,8 +4874,8 @@
     </row>
     <row r="10">
       <c r="A10" s="9"/>
-      <c r="B10" s="1" t="s">
-        <v>665</v>
+      <c r="B10" s="225" t="s">
+        <v>833</v>
       </c>
       <c r="C10" s="1">
         <v>81</v>
@@ -4590,8 +4910,8 @@
     </row>
     <row r="11">
       <c r="A11" s="9"/>
-      <c r="B11" s="1" t="s">
-        <v>666</v>
+      <c r="B11" s="225" t="s">
+        <v>834</v>
       </c>
       <c r="C11" s="1">
         <v>416</v>
@@ -4626,8 +4946,8 @@
     </row>
     <row r="12">
       <c r="A12" s="10"/>
-      <c r="B12" s="1" t="s">
-        <v>667</v>
+      <c r="B12" s="225" t="s">
+        <v>835</v>
       </c>
       <c r="C12" s="1">
         <v>100</v>
@@ -4697,7 +5017,7 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="227" t="s">
         <v>668</v>
       </c>
       <c r="C1" s="5" t="s">
@@ -4714,35 +5034,35 @@
       <c r="L1" s="7"/>
     </row>
     <row r="2">
-      <c r="C2" s="1" t="s">
-        <v>669</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>670</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>671</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>672</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>673</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>674</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>675</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>676</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>677</v>
-      </c>
-      <c r="L2" s="1" t="s">
-        <v>678</v>
+      <c r="C2" s="231" t="s">
+        <v>826</v>
+      </c>
+      <c r="D2" s="231" t="s">
+        <v>827</v>
+      </c>
+      <c r="E2" s="231" t="s">
+        <v>828</v>
+      </c>
+      <c r="F2" s="231" t="s">
+        <v>829</v>
+      </c>
+      <c r="G2" s="231" t="s">
+        <v>830</v>
+      </c>
+      <c r="H2" s="231" t="s">
+        <v>831</v>
+      </c>
+      <c r="I2" s="231" t="s">
+        <v>832</v>
+      </c>
+      <c r="J2" s="231" t="s">
+        <v>833</v>
+      </c>
+      <c r="K2" s="231" t="s">
+        <v>834</v>
+      </c>
+      <c r="L2" s="231" t="s">
+        <v>835</v>
       </c>
       <c r="N2" s="3" t="s">
         <v>4</v>
@@ -4756,8 +5076,8 @@
       <c r="A3" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>679</v>
+      <c r="B3" s="233" t="s">
+        <v>826</v>
       </c>
       <c r="C3" s="2">
         <v>83</v>
@@ -4799,8 +5119,8 @@
     </row>
     <row r="4">
       <c r="A4" s="9"/>
-      <c r="B4" s="1" t="s">
-        <v>680</v>
+      <c r="B4" s="233" t="s">
+        <v>827</v>
       </c>
       <c r="C4" s="1">
         <v>132</v>
@@ -4842,8 +5162,8 @@
     </row>
     <row r="5">
       <c r="A5" s="9"/>
-      <c r="B5" s="1" t="s">
-        <v>681</v>
+      <c r="B5" s="233" t="s">
+        <v>828</v>
       </c>
       <c r="C5" s="1">
         <v>63</v>
@@ -4878,8 +5198,8 @@
     </row>
     <row r="6">
       <c r="A6" s="9"/>
-      <c r="B6" s="1" t="s">
-        <v>682</v>
+      <c r="B6" s="233" t="s">
+        <v>829</v>
       </c>
       <c r="C6" s="1">
         <v>29</v>
@@ -4914,8 +5234,8 @@
     </row>
     <row r="7">
       <c r="A7" s="9"/>
-      <c r="B7" s="1" t="s">
-        <v>683</v>
+      <c r="B7" s="233" t="s">
+        <v>830</v>
       </c>
       <c r="C7" s="1">
         <v>37</v>
@@ -4950,8 +5270,8 @@
     </row>
     <row r="8">
       <c r="A8" s="9"/>
-      <c r="B8" s="1" t="s">
-        <v>684</v>
+      <c r="B8" s="233" t="s">
+        <v>831</v>
       </c>
       <c r="C8" s="1">
         <v>17</v>
@@ -4986,8 +5306,8 @@
     </row>
     <row r="9">
       <c r="A9" s="9"/>
-      <c r="B9" s="1" t="s">
-        <v>685</v>
+      <c r="B9" s="233" t="s">
+        <v>832</v>
       </c>
       <c r="C9" s="1">
         <v>12</v>
@@ -5022,8 +5342,8 @@
     </row>
     <row r="10">
       <c r="A10" s="9"/>
-      <c r="B10" s="1" t="s">
-        <v>686</v>
+      <c r="B10" s="233" t="s">
+        <v>833</v>
       </c>
       <c r="C10" s="1">
         <v>71</v>
@@ -5058,8 +5378,8 @@
     </row>
     <row r="11">
       <c r="A11" s="9"/>
-      <c r="B11" s="1" t="s">
-        <v>687</v>
+      <c r="B11" s="233" t="s">
+        <v>834</v>
       </c>
       <c r="C11" s="1">
         <v>103</v>
@@ -5094,8 +5414,8 @@
     </row>
     <row r="12">
       <c r="A12" s="10"/>
-      <c r="B12" s="1" t="s">
-        <v>688</v>
+      <c r="B12" s="233" t="s">
+        <v>835</v>
       </c>
       <c r="C12" s="1">
         <v>130</v>
@@ -5163,7 +5483,7 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="235" t="s">
         <v>689</v>
       </c>
       <c r="C1" s="5" t="s">
@@ -5180,35 +5500,35 @@
       <c r="L1" s="7"/>
     </row>
     <row r="2">
-      <c r="C2" s="1" t="s">
-        <v>690</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>691</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>692</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>693</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>694</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>695</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>696</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>697</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>698</v>
-      </c>
-      <c r="L2" s="1" t="s">
-        <v>699</v>
+      <c r="C2" s="239" t="s">
+        <v>826</v>
+      </c>
+      <c r="D2" s="239" t="s">
+        <v>827</v>
+      </c>
+      <c r="E2" s="239" t="s">
+        <v>828</v>
+      </c>
+      <c r="F2" s="239" t="s">
+        <v>829</v>
+      </c>
+      <c r="G2" s="239" t="s">
+        <v>830</v>
+      </c>
+      <c r="H2" s="239" t="s">
+        <v>831</v>
+      </c>
+      <c r="I2" s="239" t="s">
+        <v>832</v>
+      </c>
+      <c r="J2" s="239" t="s">
+        <v>833</v>
+      </c>
+      <c r="K2" s="239" t="s">
+        <v>834</v>
+      </c>
+      <c r="L2" s="239" t="s">
+        <v>835</v>
       </c>
       <c r="N2" s="3" t="s">
         <v>4</v>
@@ -5222,8 +5542,8 @@
       <c r="A3" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>700</v>
+      <c r="B3" s="241" t="s">
+        <v>826</v>
       </c>
       <c r="C3" s="2">
         <v>59</v>
@@ -5265,8 +5585,8 @@
     </row>
     <row r="4">
       <c r="A4" s="9"/>
-      <c r="B4" s="1" t="s">
-        <v>701</v>
+      <c r="B4" s="241" t="s">
+        <v>827</v>
       </c>
       <c r="C4" s="1">
         <v>503</v>
@@ -5308,8 +5628,8 @@
     </row>
     <row r="5">
       <c r="A5" s="9"/>
-      <c r="B5" s="1" t="s">
-        <v>702</v>
+      <c r="B5" s="241" t="s">
+        <v>828</v>
       </c>
       <c r="C5" s="1">
         <v>54</v>
@@ -5344,8 +5664,8 @@
     </row>
     <row r="6">
       <c r="A6" s="9"/>
-      <c r="B6" s="1" t="s">
-        <v>703</v>
+      <c r="B6" s="241" t="s">
+        <v>829</v>
       </c>
       <c r="C6" s="1">
         <v>29</v>
@@ -5380,8 +5700,8 @@
     </row>
     <row r="7">
       <c r="A7" s="9"/>
-      <c r="B7" s="1" t="s">
-        <v>704</v>
+      <c r="B7" s="241" t="s">
+        <v>830</v>
       </c>
       <c r="C7" s="1">
         <v>56</v>
@@ -5416,8 +5736,8 @@
     </row>
     <row r="8">
       <c r="A8" s="9"/>
-      <c r="B8" s="1" t="s">
-        <v>705</v>
+      <c r="B8" s="241" t="s">
+        <v>831</v>
       </c>
       <c r="C8" s="1">
         <v>24</v>
@@ -5452,8 +5772,8 @@
     </row>
     <row r="9">
       <c r="A9" s="9"/>
-      <c r="B9" s="1" t="s">
-        <v>706</v>
+      <c r="B9" s="241" t="s">
+        <v>832</v>
       </c>
       <c r="C9" s="1">
         <v>19</v>
@@ -5488,8 +5808,8 @@
     </row>
     <row r="10">
       <c r="A10" s="9"/>
-      <c r="B10" s="1" t="s">
-        <v>707</v>
+      <c r="B10" s="241" t="s">
+        <v>833</v>
       </c>
       <c r="C10" s="1">
         <v>57</v>
@@ -5524,8 +5844,8 @@
     </row>
     <row r="11">
       <c r="A11" s="9"/>
-      <c r="B11" s="1" t="s">
-        <v>708</v>
+      <c r="B11" s="241" t="s">
+        <v>834</v>
       </c>
       <c r="C11" s="1">
         <v>182</v>
@@ -5560,8 +5880,8 @@
     </row>
     <row r="12">
       <c r="A12" s="10"/>
-      <c r="B12" s="1" t="s">
-        <v>709</v>
+      <c r="B12" s="241" t="s">
+        <v>835</v>
       </c>
       <c r="C12" s="1">
         <v>385</v>
@@ -5630,7 +5950,7 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="243" t="s">
         <v>710</v>
       </c>
       <c r="C1" s="5" t="s">
@@ -5647,35 +5967,35 @@
       <c r="L1" s="7"/>
     </row>
     <row r="2">
-      <c r="C2" s="1" t="s">
-        <v>711</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>712</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>713</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>714</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>715</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>716</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>717</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>718</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>719</v>
-      </c>
-      <c r="L2" s="1" t="s">
-        <v>720</v>
+      <c r="C2" s="247" t="s">
+        <v>826</v>
+      </c>
+      <c r="D2" s="247" t="s">
+        <v>827</v>
+      </c>
+      <c r="E2" s="247" t="s">
+        <v>828</v>
+      </c>
+      <c r="F2" s="247" t="s">
+        <v>829</v>
+      </c>
+      <c r="G2" s="247" t="s">
+        <v>830</v>
+      </c>
+      <c r="H2" s="247" t="s">
+        <v>831</v>
+      </c>
+      <c r="I2" s="247" t="s">
+        <v>832</v>
+      </c>
+      <c r="J2" s="247" t="s">
+        <v>833</v>
+      </c>
+      <c r="K2" s="247" t="s">
+        <v>834</v>
+      </c>
+      <c r="L2" s="247" t="s">
+        <v>835</v>
       </c>
       <c r="N2" s="3" t="s">
         <v>4</v>
@@ -5689,8 +6009,8 @@
       <c r="A3" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>721</v>
+      <c r="B3" s="249" t="s">
+        <v>826</v>
       </c>
       <c r="C3" s="2">
         <v>27</v>
@@ -5732,8 +6052,8 @@
     </row>
     <row r="4">
       <c r="A4" s="9"/>
-      <c r="B4" s="1" t="s">
-        <v>722</v>
+      <c r="B4" s="249" t="s">
+        <v>827</v>
       </c>
       <c r="C4" s="1">
         <v>40</v>
@@ -5775,8 +6095,8 @@
     </row>
     <row r="5">
       <c r="A5" s="9"/>
-      <c r="B5" s="1" t="s">
-        <v>723</v>
+      <c r="B5" s="249" t="s">
+        <v>828</v>
       </c>
       <c r="C5" s="1">
         <v>57</v>
@@ -5811,8 +6131,8 @@
     </row>
     <row r="6">
       <c r="A6" s="9"/>
-      <c r="B6" s="1" t="s">
-        <v>724</v>
+      <c r="B6" s="249" t="s">
+        <v>829</v>
       </c>
       <c r="C6" s="1">
         <v>37</v>
@@ -5847,8 +6167,8 @@
     </row>
     <row r="7">
       <c r="A7" s="9"/>
-      <c r="B7" s="1" t="s">
-        <v>725</v>
+      <c r="B7" s="249" t="s">
+        <v>830</v>
       </c>
       <c r="C7" s="1">
         <v>63</v>
@@ -5883,8 +6203,8 @@
     </row>
     <row r="8">
       <c r="A8" s="9"/>
-      <c r="B8" s="1" t="s">
-        <v>726</v>
+      <c r="B8" s="249" t="s">
+        <v>831</v>
       </c>
       <c r="C8" s="1">
         <v>37</v>
@@ -5919,8 +6239,8 @@
     </row>
     <row r="9">
       <c r="A9" s="9"/>
-      <c r="B9" s="1" t="s">
-        <v>727</v>
+      <c r="B9" s="249" t="s">
+        <v>832</v>
       </c>
       <c r="C9" s="1">
         <v>45</v>
@@ -5955,8 +6275,8 @@
     </row>
     <row r="10">
       <c r="A10" s="9"/>
-      <c r="B10" s="1" t="s">
-        <v>728</v>
+      <c r="B10" s="249" t="s">
+        <v>833</v>
       </c>
       <c r="C10" s="1">
         <v>74</v>
@@ -5991,8 +6311,8 @@
     </row>
     <row r="11">
       <c r="A11" s="9"/>
-      <c r="B11" s="1" t="s">
-        <v>729</v>
+      <c r="B11" s="249" t="s">
+        <v>834</v>
       </c>
       <c r="C11" s="1">
         <v>18</v>
@@ -6027,8 +6347,8 @@
     </row>
     <row r="12">
       <c r="A12" s="10"/>
-      <c r="B12" s="1" t="s">
-        <v>730</v>
+      <c r="B12" s="249" t="s">
+        <v>835</v>
       </c>
       <c r="C12" s="1">
         <v>66</v>
@@ -6097,7 +6417,7 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="251" t="s">
         <v>731</v>
       </c>
       <c r="C1" s="5" t="s">
@@ -6114,35 +6434,35 @@
       <c r="L1" s="7"/>
     </row>
     <row r="2">
-      <c r="C2" s="1" t="s">
-        <v>732</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>733</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>734</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>735</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>736</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>737</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>738</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>739</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>740</v>
-      </c>
-      <c r="L2" s="1" t="s">
-        <v>741</v>
+      <c r="C2" s="255" t="s">
+        <v>826</v>
+      </c>
+      <c r="D2" s="255" t="s">
+        <v>827</v>
+      </c>
+      <c r="E2" s="255" t="s">
+        <v>828</v>
+      </c>
+      <c r="F2" s="255" t="s">
+        <v>829</v>
+      </c>
+      <c r="G2" s="255" t="s">
+        <v>830</v>
+      </c>
+      <c r="H2" s="255" t="s">
+        <v>831</v>
+      </c>
+      <c r="I2" s="255" t="s">
+        <v>832</v>
+      </c>
+      <c r="J2" s="255" t="s">
+        <v>833</v>
+      </c>
+      <c r="K2" s="255" t="s">
+        <v>834</v>
+      </c>
+      <c r="L2" s="255" t="s">
+        <v>835</v>
       </c>
       <c r="N2" s="3" t="s">
         <v>4</v>
@@ -6156,8 +6476,8 @@
       <c r="A3" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>742</v>
+      <c r="B3" s="257" t="s">
+        <v>826</v>
       </c>
       <c r="C3" s="2">
         <v>21</v>
@@ -6199,8 +6519,8 @@
     </row>
     <row r="4">
       <c r="A4" s="9"/>
-      <c r="B4" s="1" t="s">
-        <v>743</v>
+      <c r="B4" s="257" t="s">
+        <v>827</v>
       </c>
       <c r="C4" s="1">
         <v>35</v>
@@ -6242,8 +6562,8 @@
     </row>
     <row r="5">
       <c r="A5" s="9"/>
-      <c r="B5" s="1" t="s">
-        <v>744</v>
+      <c r="B5" s="257" t="s">
+        <v>828</v>
       </c>
       <c r="C5" s="1">
         <v>123</v>
@@ -6278,8 +6598,8 @@
     </row>
     <row r="6">
       <c r="A6" s="9"/>
-      <c r="B6" s="1" t="s">
-        <v>745</v>
+      <c r="B6" s="257" t="s">
+        <v>829</v>
       </c>
       <c r="C6" s="1">
         <v>77</v>
@@ -6314,8 +6634,8 @@
     </row>
     <row r="7">
       <c r="A7" s="9"/>
-      <c r="B7" s="1" t="s">
-        <v>746</v>
+      <c r="B7" s="257" t="s">
+        <v>830</v>
       </c>
       <c r="C7" s="1">
         <v>103</v>
@@ -6350,8 +6670,8 @@
     </row>
     <row r="8">
       <c r="A8" s="9"/>
-      <c r="B8" s="1" t="s">
-        <v>747</v>
+      <c r="B8" s="257" t="s">
+        <v>831</v>
       </c>
       <c r="C8" s="1">
         <v>89</v>
@@ -6386,8 +6706,8 @@
     </row>
     <row r="9">
       <c r="A9" s="9"/>
-      <c r="B9" s="1" t="s">
-        <v>748</v>
+      <c r="B9" s="257" t="s">
+        <v>832</v>
       </c>
       <c r="C9" s="1">
         <v>87</v>
@@ -6422,8 +6742,8 @@
     </row>
     <row r="10">
       <c r="A10" s="9"/>
-      <c r="B10" s="1" t="s">
-        <v>749</v>
+      <c r="B10" s="257" t="s">
+        <v>833</v>
       </c>
       <c r="C10" s="1">
         <v>152</v>
@@ -6458,8 +6778,8 @@
     </row>
     <row r="11">
       <c r="A11" s="9"/>
-      <c r="B11" s="1" t="s">
-        <v>750</v>
+      <c r="B11" s="257" t="s">
+        <v>834</v>
       </c>
       <c r="C11" s="1">
         <v>19</v>
@@ -6494,8 +6814,8 @@
     </row>
     <row r="12">
       <c r="A12" s="10"/>
-      <c r="B12" s="1" t="s">
-        <v>751</v>
+      <c r="B12" s="257" t="s">
+        <v>835</v>
       </c>
       <c r="C12" s="1">
         <v>52</v>
@@ -6564,7 +6884,7 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="259" t="s">
         <v>752</v>
       </c>
       <c r="C1" s="5" t="s">
@@ -6581,35 +6901,35 @@
       <c r="L1" s="7"/>
     </row>
     <row r="2">
-      <c r="C2" s="1" t="s">
-        <v>753</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>754</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>755</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>756</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>757</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>758</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>759</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>760</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>761</v>
-      </c>
-      <c r="L2" s="1" t="s">
-        <v>762</v>
+      <c r="C2" s="263" t="s">
+        <v>826</v>
+      </c>
+      <c r="D2" s="263" t="s">
+        <v>827</v>
+      </c>
+      <c r="E2" s="263" t="s">
+        <v>828</v>
+      </c>
+      <c r="F2" s="263" t="s">
+        <v>829</v>
+      </c>
+      <c r="G2" s="263" t="s">
+        <v>830</v>
+      </c>
+      <c r="H2" s="263" t="s">
+        <v>831</v>
+      </c>
+      <c r="I2" s="263" t="s">
+        <v>832</v>
+      </c>
+      <c r="J2" s="263" t="s">
+        <v>833</v>
+      </c>
+      <c r="K2" s="263" t="s">
+        <v>834</v>
+      </c>
+      <c r="L2" s="263" t="s">
+        <v>835</v>
       </c>
       <c r="N2" s="3" t="s">
         <v>4</v>
@@ -6623,8 +6943,8 @@
       <c r="A3" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>763</v>
+      <c r="B3" s="265" t="s">
+        <v>826</v>
       </c>
       <c r="C3" s="2">
         <v>32</v>
@@ -6666,8 +6986,8 @@
     </row>
     <row r="4">
       <c r="A4" s="9"/>
-      <c r="B4" s="1" t="s">
-        <v>764</v>
+      <c r="B4" s="265" t="s">
+        <v>827</v>
       </c>
       <c r="C4" s="1">
         <v>47</v>
@@ -6709,8 +7029,8 @@
     </row>
     <row r="5">
       <c r="A5" s="9"/>
-      <c r="B5" s="1" t="s">
-        <v>765</v>
+      <c r="B5" s="265" t="s">
+        <v>828</v>
       </c>
       <c r="C5" s="1">
         <v>411</v>
@@ -6745,8 +7065,8 @@
     </row>
     <row r="6">
       <c r="A6" s="9"/>
-      <c r="B6" s="1" t="s">
-        <v>766</v>
+      <c r="B6" s="265" t="s">
+        <v>829</v>
       </c>
       <c r="C6" s="1">
         <v>349</v>
@@ -6781,8 +7101,8 @@
     </row>
     <row r="7">
       <c r="A7" s="9"/>
-      <c r="B7" s="1" t="s">
-        <v>767</v>
+      <c r="B7" s="265" t="s">
+        <v>830</v>
       </c>
       <c r="C7" s="1">
         <v>558</v>
@@ -6817,8 +7137,8 @@
     </row>
     <row r="8">
       <c r="A8" s="9"/>
-      <c r="B8" s="1" t="s">
-        <v>768</v>
+      <c r="B8" s="265" t="s">
+        <v>831</v>
       </c>
       <c r="C8" s="1">
         <v>396</v>
@@ -6853,8 +7173,8 @@
     </row>
     <row r="9">
       <c r="A9" s="9"/>
-      <c r="B9" s="1" t="s">
-        <v>769</v>
+      <c r="B9" s="265" t="s">
+        <v>832</v>
       </c>
       <c r="C9" s="1">
         <v>486</v>
@@ -6889,8 +7209,8 @@
     </row>
     <row r="10">
       <c r="A10" s="9"/>
-      <c r="B10" s="1" t="s">
-        <v>770</v>
+      <c r="B10" s="265" t="s">
+        <v>833</v>
       </c>
       <c r="C10" s="1">
         <v>334</v>
@@ -6925,8 +7245,8 @@
     </row>
     <row r="11">
       <c r="A11" s="9"/>
-      <c r="B11" s="1" t="s">
-        <v>771</v>
+      <c r="B11" s="265" t="s">
+        <v>834</v>
       </c>
       <c r="C11" s="1">
         <v>22</v>
@@ -6961,8 +7281,8 @@
     </row>
     <row r="12">
       <c r="A12" s="10"/>
-      <c r="B12" s="1" t="s">
-        <v>772</v>
+      <c r="B12" s="265" t="s">
+        <v>835</v>
       </c>
       <c r="C12" s="1">
         <v>55</v>
@@ -7031,7 +7351,7 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="267" t="s">
         <v>773</v>
       </c>
       <c r="C1" s="5" t="s">
@@ -7048,35 +7368,35 @@
       <c r="L1" s="7"/>
     </row>
     <row r="2">
-      <c r="C2" s="1" t="s">
-        <v>774</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>775</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>776</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>777</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>778</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>779</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>780</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>781</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>782</v>
-      </c>
-      <c r="L2" s="1" t="s">
-        <v>783</v>
+      <c r="C2" s="271" t="s">
+        <v>826</v>
+      </c>
+      <c r="D2" s="271" t="s">
+        <v>827</v>
+      </c>
+      <c r="E2" s="271" t="s">
+        <v>828</v>
+      </c>
+      <c r="F2" s="271" t="s">
+        <v>829</v>
+      </c>
+      <c r="G2" s="271" t="s">
+        <v>830</v>
+      </c>
+      <c r="H2" s="271" t="s">
+        <v>831</v>
+      </c>
+      <c r="I2" s="271" t="s">
+        <v>832</v>
+      </c>
+      <c r="J2" s="271" t="s">
+        <v>833</v>
+      </c>
+      <c r="K2" s="271" t="s">
+        <v>834</v>
+      </c>
+      <c r="L2" s="271" t="s">
+        <v>835</v>
       </c>
       <c r="N2" s="3" t="s">
         <v>4</v>
@@ -7090,8 +7410,8 @@
       <c r="A3" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>784</v>
+      <c r="B3" s="273" t="s">
+        <v>826</v>
       </c>
       <c r="C3" s="2">
         <v>11</v>
@@ -7133,8 +7453,8 @@
     </row>
     <row r="4">
       <c r="A4" s="9"/>
-      <c r="B4" s="1" t="s">
-        <v>785</v>
+      <c r="B4" s="273" t="s">
+        <v>827</v>
       </c>
       <c r="C4" s="1">
         <v>35</v>
@@ -7176,8 +7496,8 @@
     </row>
     <row r="5">
       <c r="A5" s="9"/>
-      <c r="B5" s="1" t="s">
-        <v>786</v>
+      <c r="B5" s="273" t="s">
+        <v>828</v>
       </c>
       <c r="C5" s="1">
         <v>69</v>
@@ -7212,8 +7532,8 @@
     </row>
     <row r="6">
       <c r="A6" s="9"/>
-      <c r="B6" s="1" t="s">
-        <v>787</v>
+      <c r="B6" s="273" t="s">
+        <v>829</v>
       </c>
       <c r="C6" s="1">
         <v>177</v>
@@ -7248,8 +7568,8 @@
     </row>
     <row r="7">
       <c r="A7" s="9"/>
-      <c r="B7" s="1" t="s">
-        <v>788</v>
+      <c r="B7" s="273" t="s">
+        <v>830</v>
       </c>
       <c r="C7" s="1">
         <v>56</v>
@@ -7284,8 +7604,8 @@
     </row>
     <row r="8">
       <c r="A8" s="9"/>
-      <c r="B8" s="1" t="s">
-        <v>789</v>
+      <c r="B8" s="273" t="s">
+        <v>831</v>
       </c>
       <c r="C8" s="1">
         <v>176</v>
@@ -7320,8 +7640,8 @@
     </row>
     <row r="9">
       <c r="A9" s="9"/>
-      <c r="B9" s="1" t="s">
-        <v>790</v>
+      <c r="B9" s="273" t="s">
+        <v>832</v>
       </c>
       <c r="C9" s="1">
         <v>135</v>
@@ -7356,8 +7676,8 @@
     </row>
     <row r="10">
       <c r="A10" s="9"/>
-      <c r="B10" s="1" t="s">
-        <v>791</v>
+      <c r="B10" s="273" t="s">
+        <v>833</v>
       </c>
       <c r="C10" s="1">
         <v>113</v>
@@ -7392,8 +7712,8 @@
     </row>
     <row r="11">
       <c r="A11" s="9"/>
-      <c r="B11" s="1" t="s">
-        <v>792</v>
+      <c r="B11" s="273" t="s">
+        <v>834</v>
       </c>
       <c r="C11" s="1">
         <v>22</v>
@@ -7428,8 +7748,8 @@
     </row>
     <row r="12">
       <c r="A12" s="10"/>
-      <c r="B12" s="1" t="s">
-        <v>793</v>
+      <c r="B12" s="273" t="s">
+        <v>835</v>
       </c>
       <c r="C12" s="1">
         <v>57</v>
@@ -7498,7 +7818,7 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="275" t="s">
         <v>794</v>
       </c>
       <c r="C1" s="5" t="s">
@@ -7515,35 +7835,35 @@
       <c r="L1" s="7"/>
     </row>
     <row r="2">
-      <c r="C2" s="1" t="s">
-        <v>795</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>796</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>797</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>798</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>799</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>800</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>801</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>802</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>803</v>
-      </c>
-      <c r="L2" s="1" t="s">
-        <v>804</v>
+      <c r="C2" s="279" t="s">
+        <v>826</v>
+      </c>
+      <c r="D2" s="279" t="s">
+        <v>827</v>
+      </c>
+      <c r="E2" s="279" t="s">
+        <v>828</v>
+      </c>
+      <c r="F2" s="279" t="s">
+        <v>829</v>
+      </c>
+      <c r="G2" s="279" t="s">
+        <v>830</v>
+      </c>
+      <c r="H2" s="279" t="s">
+        <v>831</v>
+      </c>
+      <c r="I2" s="279" t="s">
+        <v>832</v>
+      </c>
+      <c r="J2" s="279" t="s">
+        <v>833</v>
+      </c>
+      <c r="K2" s="279" t="s">
+        <v>834</v>
+      </c>
+      <c r="L2" s="279" t="s">
+        <v>835</v>
       </c>
       <c r="N2" s="3" t="s">
         <v>4</v>
@@ -7557,8 +7877,8 @@
       <c r="A3" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>805</v>
+      <c r="B3" s="281" t="s">
+        <v>826</v>
       </c>
       <c r="C3" s="2">
         <v>13</v>
@@ -7600,8 +7920,8 @@
     </row>
     <row r="4">
       <c r="A4" s="9"/>
-      <c r="B4" s="1" t="s">
-        <v>806</v>
+      <c r="B4" s="281" t="s">
+        <v>827</v>
       </c>
       <c r="C4" s="1">
         <v>36</v>
@@ -7643,8 +7963,8 @@
     </row>
     <row r="5">
       <c r="A5" s="9"/>
-      <c r="B5" s="1" t="s">
-        <v>807</v>
+      <c r="B5" s="281" t="s">
+        <v>828</v>
       </c>
       <c r="C5" s="1">
         <v>57</v>
@@ -7679,8 +7999,8 @@
     </row>
     <row r="6">
       <c r="A6" s="9"/>
-      <c r="B6" s="1" t="s">
-        <v>808</v>
+      <c r="B6" s="281" t="s">
+        <v>829</v>
       </c>
       <c r="C6" s="1">
         <v>132</v>
@@ -7715,8 +8035,8 @@
     </row>
     <row r="7">
       <c r="A7" s="9"/>
-      <c r="B7" s="1" t="s">
-        <v>809</v>
+      <c r="B7" s="281" t="s">
+        <v>830</v>
       </c>
       <c r="C7" s="1">
         <v>33</v>
@@ -7751,8 +8071,8 @@
     </row>
     <row r="8">
       <c r="A8" s="9"/>
-      <c r="B8" s="1" t="s">
-        <v>810</v>
+      <c r="B8" s="281" t="s">
+        <v>831</v>
       </c>
       <c r="C8" s="1">
         <v>116</v>
@@ -7787,8 +8107,8 @@
     </row>
     <row r="9">
       <c r="A9" s="9"/>
-      <c r="B9" s="1" t="s">
-        <v>811</v>
+      <c r="B9" s="281" t="s">
+        <v>832</v>
       </c>
       <c r="C9" s="1">
         <v>111</v>
@@ -7823,8 +8143,8 @@
     </row>
     <row r="10">
       <c r="A10" s="9"/>
-      <c r="B10" s="1" t="s">
-        <v>812</v>
+      <c r="B10" s="281" t="s">
+        <v>833</v>
       </c>
       <c r="C10" s="1">
         <v>58</v>
@@ -7859,8 +8179,8 @@
     </row>
     <row r="11">
       <c r="A11" s="9"/>
-      <c r="B11" s="1" t="s">
-        <v>813</v>
+      <c r="B11" s="281" t="s">
+        <v>834</v>
       </c>
       <c r="C11" s="1">
         <v>14</v>
@@ -7895,8 +8215,8 @@
     </row>
     <row r="12">
       <c r="A12" s="10"/>
-      <c r="B12" s="1" t="s">
-        <v>814</v>
+      <c r="B12" s="281" t="s">
+        <v>835</v>
       </c>
       <c r="C12" s="1">
         <v>41</v>

</xml_diff>